<commit_message>
Stats: cli graphs and updated overview
</commit_message>
<xml_diff>
--- a/defects4j_benchmark.xlsx
+++ b/defects4j_benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D771C364-88ED-4D8D-B91B-F54C69649DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1BB3FF-14D7-4A4C-BDDD-46C7FC04FE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2550" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
+    <workbookView xWindow="7005" yWindow="1455" windowWidth="20415" windowHeight="14475" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
     <t>4h</t>
   </si>
   <si>
-    <t>x</t>
+    <t>OOM</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,13 +717,13 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -806,10 +806,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Stats: gson graphs and updated overview
</commit_message>
<xml_diff>
--- a/defects4j_benchmark.xlsx
+++ b/defects4j_benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1BB3FF-14D7-4A4C-BDDD-46C7FC04FE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CADD5D0-D315-4244-BBDE-8109CC9F0ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="1455" windowWidth="20415" windowHeight="14475" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
+    <workbookView xWindow="-28920" yWindow="3315" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,13 +717,13 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>3</v>

</xml_diff>

<commit_message>
Stats: only evaluate relevant fields in sheet (prevents OOM)
</commit_message>
<xml_diff>
--- a/defects4j_benchmark.xlsx
+++ b/defects4j_benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674229DE-7889-4787-8B9C-2C0F49729F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0BA009-4E55-4BD6-83A2-3A673C747433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
+    <workbookView xWindow="38280" yWindow="-4515" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A6D3405A-B8B7-4A98-A54C-07860933E086}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -679,7 +679,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +779,15 @@
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -821,6 +830,12 @@
       </c>
       <c r="F5" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
       <c r="K5" s="4"/>
     </row>

</xml_diff>